<commit_message>
update augumentation to simuulate cornneal reflection
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="26">
   <si>
     <t>Segmentation + Center</t>
     <phoneticPr fontId="1"/>
@@ -114,7 +114,20 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>checkpoints_fcn00.augumented</t>
+    <t>NNLAB: Estimated 36/48</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NNLAB: Estimated 39 / 48</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NNLAB: estimated 39/48</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NNLAB: Estimated 41/48</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -435,7 +448,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -505,18 +518,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -531,6 +544,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D845C81D-AC18-429C-8E31-5822E06AF031}">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1063,7 +1079,7 @@
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="11.75" customWidth="1"/>
     <col min="8" max="8" width="12.125" customWidth="1"/>
@@ -1114,7 +1130,7 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1130,7 +1146,7 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1143,16 +1159,22 @@
       <c r="E4" s="21">
         <v>6.4975000000000005E-2</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="5">
+        <v>0.56208599999999997</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2.3933610000000001</v>
+      </c>
+      <c r="H4" s="32">
+        <v>-0.56828199999999995</v>
+      </c>
       <c r="I4" s="13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1166,7 +1188,7 @@
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1180,7 +1202,7 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1216,7 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1230,7 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1226,7 +1248,7 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="25"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1264,7 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="25"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1256,7 +1278,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -1270,7 +1292,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="25"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1306,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="25"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1298,7 +1320,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1324,7 +1346,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="25"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1370,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1384,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" s="25"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1398,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
@@ -1390,7 +1412,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="26"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
@@ -1458,7 +1480,7 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1474,7 +1496,7 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" s="24"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="4" t="s">
         <v>2</v>
       </c>
@@ -1487,14 +1509,22 @@
       <c r="E25" s="21">
         <v>-0.13662099999999999</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="13"/>
+      <c r="F25" s="5">
+        <v>0.54704799999999998</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2.2653979999999998</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-0.62666500000000003</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A26" s="24"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
@@ -1508,7 +1538,7 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A27" s="24"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
@@ -1522,7 +1552,7 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A28" s="24"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="4" t="s">
         <v>5</v>
       </c>
@@ -1536,7 +1566,7 @@
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="24"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
         <v>6</v>
       </c>
@@ -1550,7 +1580,7 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1568,7 +1598,7 @@
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="25"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>2</v>
       </c>
@@ -1584,7 +1614,7 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="25"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="4" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1628,7 @@
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="25"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>4</v>
       </c>
@@ -1612,7 +1642,7 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="25"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
@@ -1626,7 +1656,7 @@
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:10" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="25"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="10" t="s">
         <v>6</v>
       </c>
@@ -1640,7 +1670,7 @@
       <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1664,7 +1694,7 @@
       <c r="J36" s="5"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A37" s="25"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="5" t="s">
         <v>2</v>
       </c>
@@ -1688,7 +1718,7 @@
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A38" s="25"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1732,7 @@
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A39" s="25"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="5" t="s">
         <v>4</v>
       </c>
@@ -1716,7 +1746,7 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A40" s="25"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="5" t="s">
         <v>5</v>
       </c>
@@ -1730,7 +1760,7 @@
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="26"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="8" t="s">
         <v>6</v>
       </c>
@@ -1786,7 +1816,7 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -1802,7 +1832,7 @@
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A45" s="24"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="4" t="s">
         <v>2</v>
       </c>
@@ -1815,18 +1845,22 @@
       <c r="E45" s="21">
         <v>0.12975800000000001</v>
       </c>
-      <c r="F45" s="5"/>
+      <c r="F45" s="5">
+        <v>0.481323</v>
+      </c>
       <c r="G45" s="5">
-        <v>27.196380999999999</v>
+        <v>2.0770569999999999</v>
       </c>
       <c r="H45" s="5">
-        <v>15.750921999999999</v>
-      </c>
-      <c r="I45" s="13"/>
+        <v>-0.62484499999999998</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A46" s="24"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="4" t="s">
         <v>3</v>
       </c>
@@ -1840,7 +1874,7 @@
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A47" s="24"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="4" t="s">
         <v>4</v>
       </c>
@@ -1854,7 +1888,7 @@
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A48" s="24"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="4" t="s">
         <v>5</v>
       </c>
@@ -1868,7 +1902,7 @@
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="24"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="10" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1916,7 @@
       <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1900,7 +1934,7 @@
       <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="25"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="4" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +1950,7 @@
       <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="25"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="4" t="s">
         <v>3</v>
       </c>
@@ -1930,7 +1964,7 @@
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="25"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="4" t="s">
         <v>4</v>
       </c>
@@ -1944,7 +1978,7 @@
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="25"/>
+      <c r="A54" s="23"/>
       <c r="B54" s="4" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +1992,7 @@
       <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="25"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="10" t="s">
         <v>6</v>
       </c>
@@ -1972,7 +2006,7 @@
       <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -1996,7 +2030,7 @@
       <c r="J56" s="5"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A57" s="25"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="5" t="s">
         <v>2</v>
       </c>
@@ -2009,10 +2043,10 @@
       </c>
       <c r="F57" s="5"/>
       <c r="G57">
-        <v>-7.9573099999999997</v>
+        <v>2.754143</v>
       </c>
       <c r="H57">
-        <v>-1.752535</v>
+        <v>-0.65172699999999995</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>19</v>
@@ -2020,7 +2054,7 @@
       <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A58" s="25"/>
+      <c r="A58" s="23"/>
       <c r="B58" s="5" t="s">
         <v>3</v>
       </c>
@@ -2034,7 +2068,7 @@
       <c r="J58" s="5"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A59" s="25"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="5" t="s">
         <v>4</v>
       </c>
@@ -2048,7 +2082,7 @@
       <c r="J59" s="5"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A60" s="25"/>
+      <c r="A60" s="23"/>
       <c r="B60" s="5" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2096,7 @@
       <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="26"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="8" t="s">
         <v>6</v>
       </c>
@@ -2147,11 +2181,17 @@
       <c r="E66">
         <v>-0.27750799999999998</v>
       </c>
+      <c r="F66">
+        <v>0.481323</v>
+      </c>
       <c r="G66">
-        <v>23.497805</v>
+        <v>2.754143</v>
       </c>
       <c r="H66">
-        <v>13.524773</v>
+        <v>-0.65172699999999995</v>
+      </c>
+      <c r="I66" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.4">
@@ -2291,7 +2331,7 @@
       <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -2314,7 +2354,7 @@
       <c r="I77" s="13"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A78" s="25"/>
+      <c r="A78" s="23"/>
       <c r="B78" s="5" t="s">
         <v>2</v>
       </c>
@@ -2337,7 +2377,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A79" s="25"/>
+      <c r="A79" s="23"/>
       <c r="B79" s="5" t="s">
         <v>3</v>
       </c>
@@ -2350,7 +2390,7 @@
       <c r="I79" s="13"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A80" s="25"/>
+      <c r="A80" s="23"/>
       <c r="B80" s="5" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2403,7 @@
       <c r="I80" s="13"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A81" s="25"/>
+      <c r="A81" s="23"/>
       <c r="B81" s="5" t="s">
         <v>5</v>
       </c>
@@ -2376,7 +2416,7 @@
       <c r="I81" s="13"/>
     </row>
     <row r="82" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="26"/>
+      <c r="A82" s="24"/>
       <c r="B82" s="8" t="s">
         <v>6</v>
       </c>
@@ -2395,18 +2435,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A20"/>
     <mergeCell ref="A77:A82"/>
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="A50:A55"/>
     <mergeCell ref="A65:A70"/>
     <mergeCell ref="A71:A76"/>
     <mergeCell ref="A56:A61"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>